<commit_message>
- updates for - Remove receipt that is automatically sent to health partners - Development Request: Update logic for lite plan - Development Request: Create a drop down option in Dependent - Download In-Network and Out-of-Network transactions csv
</commit_message>
<xml_diff>
--- a/public/excel/Employees and Dependents.xlsx
+++ b/public/excel/Employees and Dependents.xlsx
@@ -206,8 +206,8 @@
   </sheetPr>
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X:X"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -345,6 +345,28 @@
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <dataValidations count="5">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L1" type="list">
+      <formula1>"Spouse,Child,Sibling,Parent,Family"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O1" type="list">
+      <formula1>"Spouse,Child,Sibling,Parent,Family"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R1" type="list">
+      <formula1>"Spouse,Child,Sibling,Parent,Family"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U1" type="list">
+      <formula1>"Spouse,Child,Sibling,Parent,Family"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X1" type="list">
+      <formula1>"Spouse,Child,Sibling,Parent,Family"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>